<commit_message>
ubo and directory done
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/barlintestinvalidData.xlsx
+++ b/src/test/resources/testdata/barlintestinvalidData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\barlinendto end\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325553BE-3975-486E-B167-7A98A404B7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22122194-15E0-4506-8F94-D6E296028CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F104BCDF-07CE-E345-81D9-603FD5D8F11E}"/>
   </bookViews>
@@ -16,8 +16,10 @@
     <sheet name="personal data" sheetId="1" r:id="rId1"/>
     <sheet name="BInformation" sheetId="3" r:id="rId2"/>
     <sheet name="Business Address" sheetId="5" r:id="rId3"/>
+    <sheet name="UBOs" sheetId="6" r:id="rId4"/>
+    <sheet name="Directors" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>dob</t>
   </si>
@@ -227,6 +229,84 @@
   </si>
   <si>
     <t>SGST1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Nationality is required.</t>
+  </si>
+  <si>
+    <t>Identity number is required.</t>
+  </si>
+  <si>
+    <t>countyValidation</t>
+  </si>
+  <si>
+    <t>uboNoValidation</t>
+  </si>
+  <si>
+    <t>uboAddressValidation</t>
+  </si>
+  <si>
+    <t>uboPercentageValidation</t>
+  </si>
+  <si>
+    <t>uboIdentityNumber</t>
+  </si>
+  <si>
+    <t>uboAddress</t>
+  </si>
+  <si>
+    <t>uboPercentage</t>
+  </si>
+  <si>
+    <t>22, Choyangmen</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Identity number should be at least 5 characters long.</t>
+  </si>
+  <si>
+    <t>Full address is required.</t>
+  </si>
+  <si>
+    <t>22 test</t>
+  </si>
+  <si>
+    <t>Full address should be at least 10 characters long.</t>
+  </si>
+  <si>
+    <t>test22, Choyangmen</t>
+  </si>
+  <si>
+    <t>Percentage of ownership is required.</t>
+  </si>
+  <si>
+    <t>Percentage of ownership must be 25 or greater.</t>
+  </si>
+  <si>
+    <t>Directors are required.</t>
+  </si>
+  <si>
+    <t>directorsValidation</t>
+  </si>
+  <si>
+    <t>directorIdentityNumber</t>
+  </si>
+  <si>
+    <t>directorINoValidation</t>
+  </si>
+  <si>
+    <t>addressOfResidence</t>
+  </si>
+  <si>
+    <t>directorAddressValidation</t>
+  </si>
+  <si>
+    <t>22, Choyangmen test</t>
   </si>
 </sst>
 </file>
@@ -598,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D30B302-4260-D743-ABB2-24C949779D5A}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1014,7 +1094,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1098,7 +1178,9 @@
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1153,4 +1235,298 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C70FFBF-3649-432A-A5C6-0738C8909079}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.09765625" customWidth="1"/>
+    <col min="2" max="2" width="27.69921875" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" customWidth="1"/>
+    <col min="4" max="4" width="31.796875" customWidth="1"/>
+    <col min="5" max="5" width="20.8984375" customWidth="1"/>
+    <col min="6" max="6" width="53.796875" customWidth="1"/>
+    <col min="7" max="7" width="49.3984375" customWidth="1"/>
+    <col min="8" max="8" width="50.3984375" customWidth="1"/>
+    <col min="9" max="9" width="24.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>123456789</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5">
+        <v>123456</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
+        <v>123456</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>123456</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8">
+        <v>123456</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9">
+        <v>123456</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97317264-D431-4F41-B27D-CFC3EBF50202}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" activeCellId="1" sqref="A7 D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.8984375" customWidth="1"/>
+    <col min="2" max="2" width="34.3984375" customWidth="1"/>
+    <col min="3" max="3" width="23.69921875" customWidth="1"/>
+    <col min="4" max="4" width="34.8984375" customWidth="1"/>
+    <col min="5" max="5" width="49.3984375" customWidth="1"/>
+    <col min="6" max="6" width="45.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>123456789</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5">
+        <v>123456789</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
+        <v>123456789</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>123456789</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>